<commit_message>
Updated Sprint 2 backlog for day 1 progress
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Documents/Agile_Development_Project1/Sprint 2/Sprint_Backlog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kamila/Documents/AppliedComp/Agile/Agile_Development_Project1/Sprint 2/Sprint_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32026CE5-8E5D-4B48-AC2A-5A88F5379B07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B87DAB-0215-764C-A408-361D2BA7D775}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Sprint 2 Backlog" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="42">
   <si>
     <t>AGILE SPRINT BACKLOG TEMPLATE WITH BURNDOWN CHART</t>
   </si>
@@ -155,6 +153,9 @@
   <si>
     <t>As a user, I can search based on location input</t>
   </si>
+  <si>
+    <t>IN progress</t>
+  </si>
 </sst>
 </file>
 
@@ -170,60 +171,71 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="22"/>
       <color rgb="FF7F7F7F"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="21"/>
       <color rgb="FF7F7F7F"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="22"/>
       <color theme="0"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -515,7 +527,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
   <c:style val="2"/>
   <c:chart>
@@ -582,10 +594,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Agile Sprint 2 Backlog'!$H$4:$M$4</c:f>
+              <c:f>'Agile Sprint 2 Backlog'!$H$15:$M$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -989,9 +1019,9 @@
   </sheetPr>
   <dimension ref="A1:AC991"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1121,7 +1151,9 @@
       <c r="G3" s="15">
         <v>3</v>
       </c>
-      <c r="H3" s="13"/>
+      <c r="H3" s="15">
+        <v>3</v>
+      </c>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -1165,7 +1197,9 @@
       <c r="G4" s="9">
         <v>5</v>
       </c>
-      <c r="H4" s="10"/>
+      <c r="H4" s="10">
+        <v>5</v>
+      </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -1209,7 +1243,9 @@
       <c r="G5" s="12">
         <v>2</v>
       </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="13">
+        <v>2</v>
+      </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
@@ -1241,7 +1277,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>24</v>
@@ -1253,7 +1289,9 @@
       <c r="G6" s="12">
         <v>8</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="13">
+        <v>7</v>
+      </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
@@ -1284,8 +1322,8 @@
       <c r="B7" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>17</v>
+      <c r="C7" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D7" s="30" t="s">
         <v>26</v>
@@ -1297,7 +1335,9 @@
       <c r="G7" s="15">
         <v>3</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="13">
+        <v>1</v>
+      </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
@@ -1341,7 +1381,9 @@
       <c r="G8" s="12">
         <v>5</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="13">
+        <v>5</v>
+      </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
@@ -1373,7 +1415,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>20</v>
@@ -1385,7 +1427,9 @@
       <c r="G9" s="12">
         <v>5</v>
       </c>
-      <c r="H9" s="13"/>
+      <c r="H9" s="13">
+        <v>4</v>
+      </c>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
@@ -1429,7 +1473,9 @@
       <c r="G10" s="12">
         <v>1</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -1473,7 +1519,9 @@
       <c r="G11" s="12">
         <v>2</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="13">
+        <v>2</v>
+      </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
@@ -1517,7 +1565,9 @@
       <c r="G12" s="15">
         <v>5</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="13">
+        <v>5</v>
+      </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -1561,7 +1611,9 @@
       <c r="G13" s="15">
         <v>3</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="13">
+        <v>2</v>
+      </c>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
@@ -1605,7 +1657,9 @@
       <c r="G14" s="15">
         <v>5</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="13">
+        <v>4</v>
+      </c>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
@@ -1638,19 +1692,19 @@
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16">
-        <f>SUM(G4:G11)</f>
-        <v>31</v>
+        <f>SUM(G3:G14)</f>
+        <v>47</v>
       </c>
       <c r="H15" s="16">
-        <f>SUM(H5:H11)</f>
-        <v>0</v>
+        <f>SUM(H3:H14)</f>
+        <v>41</v>
       </c>
       <c r="I15" s="16">
-        <f>SUM(I4:I11)</f>
+        <f>SUM(I3:I14)</f>
         <v>0</v>
       </c>
       <c r="J15" s="16">
-        <f>SUM(J4:J11)</f>
+        <f>SUM(J3:J14)</f>
         <v>0</v>
       </c>
       <c r="K15" s="16">

</xml_diff>

<commit_message>
Updated sprint 2 backlog to reflect day 2 progress
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kamila/Documents/AppliedComp/Agile/Agile_Development_Project1/Sprint 2/Sprint_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B87DAB-0215-764C-A408-361D2BA7D775}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3CE5AF-EA56-EA4E-9260-06A8A49FF652}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
   <si>
     <t>AGILE SPRINT BACKLOG TEMPLATE WITH BURNDOWN CHART</t>
   </si>
@@ -602,7 +602,7 @@
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1019,7 +1019,7 @@
   </sheetPr>
   <dimension ref="A1:AC991"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
@@ -1154,7 +1154,9 @@
       <c r="H3" s="15">
         <v>3</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="13">
+        <v>3</v>
+      </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
@@ -1200,7 +1202,9 @@
       <c r="H4" s="10">
         <v>5</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10">
+        <v>5</v>
+      </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
@@ -1236,7 +1240,9 @@
       <c r="D5" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="19"/>
+      <c r="E5" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="F5" s="12">
         <v>6</v>
       </c>
@@ -1246,7 +1252,9 @@
       <c r="H5" s="13">
         <v>2</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="I5" s="13">
+        <v>0</v>
+      </c>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
@@ -1292,7 +1300,9 @@
       <c r="H6" s="13">
         <v>7</v>
       </c>
-      <c r="I6" s="13"/>
+      <c r="I6" s="13">
+        <v>5</v>
+      </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
@@ -1338,7 +1348,9 @@
       <c r="H7" s="13">
         <v>1</v>
       </c>
-      <c r="I7" s="13"/>
+      <c r="I7" s="13">
+        <v>1</v>
+      </c>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
@@ -1384,7 +1396,9 @@
       <c r="H8" s="13">
         <v>5</v>
       </c>
-      <c r="I8" s="13"/>
+      <c r="I8" s="13">
+        <v>5</v>
+      </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -1430,7 +1444,9 @@
       <c r="H9" s="13">
         <v>4</v>
       </c>
-      <c r="I9" s="13"/>
+      <c r="I9" s="13">
+        <v>4</v>
+      </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -1476,7 +1492,9 @@
       <c r="H10" s="13">
         <v>1</v>
       </c>
-      <c r="I10" s="13"/>
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -1522,7 +1540,9 @@
       <c r="H11" s="13">
         <v>2</v>
       </c>
-      <c r="I11" s="13"/>
+      <c r="I11" s="13">
+        <v>2</v>
+      </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -1568,7 +1588,9 @@
       <c r="H12" s="13">
         <v>5</v>
       </c>
-      <c r="I12" s="13"/>
+      <c r="I12" s="13">
+        <v>4</v>
+      </c>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -1614,7 +1636,9 @@
       <c r="H13" s="13">
         <v>2</v>
       </c>
-      <c r="I13" s="13"/>
+      <c r="I13" s="13">
+        <v>2</v>
+      </c>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -1660,7 +1684,9 @@
       <c r="H14" s="13">
         <v>4</v>
       </c>
-      <c r="I14" s="13"/>
+      <c r="I14" s="13">
+        <v>3</v>
+      </c>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
@@ -1701,7 +1727,7 @@
       </c>
       <c r="I15" s="16">
         <f>SUM(I3:I14)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J15" s="16">
         <f>SUM(J3:J14)</f>

</xml_diff>

<commit_message>
minor change to srpint 2 backlog
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kamila/Documents/AppliedComp/Agile/Agile_Development_Project1/Sprint 2/Sprint_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3CE5AF-EA56-EA4E-9260-06A8A49FF652}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D8C045-378F-8B4F-89C5-E2EF4517C845}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="43">
   <si>
     <t>AGILE SPRINT BACKLOG TEMPLATE WITH BURNDOWN CHART</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>IN progress</t>
+  </si>
+  <si>
+    <t>As a programmer, I want to host the website on the server</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Agile Sprint 2 Backlog'!$H$15:$M$15</c:f>
+              <c:f>'Agile Sprint 2 Backlog'!$H$16:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1017,11 +1020,11 @@
     <tabColor rgb="FF44546A"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC991"/>
+  <dimension ref="A1:AC992"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18:W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1132,7 +1135,7 @@
     </row>
     <row r="3" spans="1:29" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
-        <f t="shared" ref="A3:A14" si="0">ROW()-2</f>
+        <f t="shared" ref="A3:A15" si="0">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" s="32" t="s">
@@ -1708,84 +1711,101 @@
       <c r="AB14" s="14"/>
       <c r="AC14" s="14"/>
     </row>
-    <row r="15" spans="1:29" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="16" t="s">
+    <row r="15" spans="1:29" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="15">
+        <v>10</v>
+      </c>
+      <c r="G15" s="15">
+        <v>5</v>
+      </c>
+      <c r="H15" s="13">
+        <v>5</v>
+      </c>
+      <c r="I15" s="13">
+        <v>4</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+    </row>
+    <row r="16" spans="1:29" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16">
         <f>SUM(G3:G14)</f>
         <v>47</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H16" s="16">
         <f>SUM(H3:H14)</f>
         <v>41</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I16" s="16">
         <f>SUM(I3:I14)</f>
         <v>35</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J16" s="16">
         <f>SUM(J3:J14)</f>
         <v>0</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K16" s="16">
         <f>SUM(K4:K11)</f>
         <v>0</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L16" s="16">
         <f>SUM(L4:L11)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M16" s="16">
         <f>SUM(M4:M11)</f>
         <v>0</v>
       </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-    </row>
-    <row r="16" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="22"/>
-      <c r="U16" s="22"/>
-      <c r="V16" s="22"/>
-      <c r="W16" s="22"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
@@ -1793,30 +1813,30 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
     </row>
-    <row r="17" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="40"/>
-      <c r="T17" s="40"/>
-      <c r="U17" s="40"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="40"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
@@ -1824,30 +1844,30 @@
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
     </row>
-    <row r="18" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="22"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
@@ -1860,7 +1880,7 @@
       <c r="B19" s="22"/>
       <c r="C19" s="23"/>
       <c r="D19" s="22"/>
-      <c r="E19" s="25"/>
+      <c r="E19" s="24"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
@@ -1879,7 +1899,7 @@
       <c r="U19" s="22"/>
       <c r="V19" s="22"/>
       <c r="W19" s="22"/>
-      <c r="X19" s="20"/>
+      <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -1888,29 +1908,29 @@
     </row>
     <row r="20" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="22"/>
+      <c r="X20" s="20"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -4740,34 +4760,34 @@
     </row>
     <row r="112" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="18"/>
-      <c r="D112" s="1"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="2"/>
       <c r="E112" s="20"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
-      <c r="I112" s="1"/>
-      <c r="J112" s="1"/>
-      <c r="K112" s="1"/>
-      <c r="L112" s="1"/>
-      <c r="M112" s="1"/>
-      <c r="N112" s="1"/>
-      <c r="O112" s="1"/>
-      <c r="P112" s="1"/>
-      <c r="Q112" s="1"/>
-      <c r="R112" s="1"/>
-      <c r="S112" s="1"/>
-      <c r="T112" s="1"/>
-      <c r="U112" s="1"/>
-      <c r="V112" s="1"/>
-      <c r="W112" s="1"/>
-      <c r="X112" s="1"/>
-      <c r="Y112" s="1"/>
-      <c r="Z112" s="1"/>
-      <c r="AA112" s="1"/>
-      <c r="AB112" s="1"/>
-      <c r="AC112" s="1"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+      <c r="K112" s="2"/>
+      <c r="L112" s="2"/>
+      <c r="M112" s="2"/>
+      <c r="N112" s="2"/>
+      <c r="O112" s="2"/>
+      <c r="P112" s="2"/>
+      <c r="Q112" s="2"/>
+      <c r="R112" s="2"/>
+      <c r="S112" s="2"/>
+      <c r="T112" s="2"/>
+      <c r="U112" s="2"/>
+      <c r="V112" s="2"/>
+      <c r="W112" s="2"/>
+      <c r="X112" s="2"/>
+      <c r="Y112" s="2"/>
+      <c r="Z112" s="2"/>
+      <c r="AA112" s="2"/>
+      <c r="AB112" s="2"/>
+      <c r="AC112" s="2"/>
     </row>
     <row r="113" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
@@ -4867,7 +4887,7 @@
       <c r="B116" s="1"/>
       <c r="C116" s="18"/>
       <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
+      <c r="E116" s="20"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
@@ -31894,8 +31914,36 @@
       <c r="AB987" s="1"/>
       <c r="AC987" s="1"/>
     </row>
-    <row r="988" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="988" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A988" s="1"/>
+      <c r="B988" s="1"/>
+      <c r="C988" s="18"/>
+      <c r="D988" s="1"/>
       <c r="E988" s="1"/>
+      <c r="F988" s="1"/>
+      <c r="G988" s="1"/>
+      <c r="H988" s="1"/>
+      <c r="I988" s="1"/>
+      <c r="J988" s="1"/>
+      <c r="K988" s="1"/>
+      <c r="L988" s="1"/>
+      <c r="M988" s="1"/>
+      <c r="N988" s="1"/>
+      <c r="O988" s="1"/>
+      <c r="P988" s="1"/>
+      <c r="Q988" s="1"/>
+      <c r="R988" s="1"/>
+      <c r="S988" s="1"/>
+      <c r="T988" s="1"/>
+      <c r="U988" s="1"/>
+      <c r="V988" s="1"/>
+      <c r="W988" s="1"/>
+      <c r="X988" s="1"/>
+      <c r="Y988" s="1"/>
+      <c r="Z988" s="1"/>
+      <c r="AA988" s="1"/>
+      <c r="AB988" s="1"/>
+      <c r="AC988" s="1"/>
     </row>
     <row r="989" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E989" s="1"/>
@@ -31905,11 +31953,14 @@
     </row>
     <row r="991" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E991" s="1"/>
+    </row>
+    <row r="992" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E992" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:W1"/>
-    <mergeCell ref="B17:W17"/>
+    <mergeCell ref="B18:W18"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup fitToHeight="0" orientation="landscape"/>

</xml_diff>